<commit_message>
Multiple Hobbies update complete
</commit_message>
<xml_diff>
--- a/data1.xlsx
+++ b/data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\UserAuthentication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D9514D-6854-4C4D-852F-823C6BFFA8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DC9617-A3FE-4899-8F0C-9FFF6F68C376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12624" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,22 +43,22 @@
     <t>hobbies</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
     <t>gujarat</t>
   </si>
   <si>
-    <t>test3@gmail.com</t>
-  </si>
-  <si>
-    <t>DEV</t>
-  </si>
-  <si>
-    <t>Dance</t>
-  </si>
-  <si>
     <t>BHUJ</t>
+  </si>
+  <si>
+    <t>Reading,Watching Movies</t>
+  </si>
+  <si>
+    <t>Mili</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>mili@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="14.4"/>
@@ -441,19 +441,19 @@
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>